<commit_message>
edit yaparken anlık olarak zemin rengi değişmesi eklendi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/FM-08-MKDGCrankPinMeasurementForm(2).xlsx
+++ b/WebApplication1/Forms/FM-08-MKDGCrankPinMeasurementForm(2).xlsx
@@ -631,8 +631,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1213,6 +1214,22 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1300,22 +1317,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1794,34 +1795,34 @@
       <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="32"/>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
@@ -1840,65 +1841,65 @@
       <c r="F4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="57"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="33"/>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="44" t="s">
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="40"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:11" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="49"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="65"/>
-      <c r="G7" s="36" t="s">
+      <c r="E7" s="36"/>
+      <c r="G7" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="15" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="68"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
@@ -2001,24 +2002,24 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="2"/>
       <c r="D14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="66"/>
-      <c r="G14" s="36" t="s">
+      <c r="E14" s="37"/>
+      <c r="G14" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="37"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="2"/>
       <c r="J14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="67"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
@@ -2122,24 +2123,24 @@
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="37"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="11"/>
       <c r="D21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="67"/>
-      <c r="G21" s="36" t="s">
+      <c r="E21" s="38"/>
+      <c r="G21" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="2"/>
       <c r="J21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K21" s="67"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
@@ -2244,49 +2245,49 @@
       <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
     </row>
     <row r="30" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -2295,34 +2296,34 @@
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="50" t="s">
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="62"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
     </row>
     <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
@@ -2332,219 +2333,219 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
-      <c r="K36" s="63"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
     </row>
     <row r="37" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
     </row>
     <row r="39" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
     </row>
     <row r="40" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
     </row>
     <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="50"/>
     </row>
     <row r="43" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
     </row>
     <row r="46" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
     </row>
     <row r="47" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
     </row>
     <row r="48" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
     </row>
     <row r="49" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
-      <c r="K49" s="38"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="17"/>
@@ -2563,14 +2564,14 @@
       <c r="A51" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="60" t="s">
+      <c r="B51" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="16"/>
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
@@ -2621,65 +2622,65 @@
       <c r="A55" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="58" t="s">
+      <c r="B55" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62"/>
     </row>
     <row r="56" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
-      <c r="J56" s="58"/>
-      <c r="K56" s="58"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="42" t="s">
+      <c r="A57" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="41"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="42"/>
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="41"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -2724,10 +2725,6 @@
     <mergeCell ref="A46:K46"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="date" showErrorMessage="1" errorTitle="test" error="bu kısıma tarih girilmelidir, boş olamaz." prompt="bu kısıma tarih girilmelidir, boş olamaz" sqref="K1">
-      <formula1>1</formula1>
-      <formula2>73051</formula2>
-    </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3:B5">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -2743,6 +2740,9 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="E9:E12 E16:E19 E23:E26 K9:K12 K16:K19 K23:K26">
       <formula1>1</formula1>
     </dataValidation>
+    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="K1">
+      <formula1>43831</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.3125" right="4.1666666666666664E-2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>